<commit_message>
added mouse feedback and absent trials
</commit_message>
<xml_diff>
--- a/chooseBlocks.xlsx
+++ b/chooseBlocks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcin\Desktop\simpleConjunction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58EB12B5-04B7-4DC8-8CB9-7B4DEC079BF3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{723FB323-952F-4B25-A44F-904B4E6C8A70}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30405" yWindow="3465" windowWidth="25590" windowHeight="12225" xr2:uid="{8EE45817-3F1D-4ED5-AA56-A662518BD526}"/>
+    <workbookView xWindow="2505" yWindow="840" windowWidth="25590" windowHeight="12225" xr2:uid="{8EE45817-3F1D-4ED5-AA56-A662518BD526}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,10 +56,10 @@
     <t>instructionText</t>
   </si>
   <si>
-    <t>Look for red horizontal target. When you find it press SPACE bar. When the search array disappears click with mouse coursor where the target was. Press SPACE to start.</t>
-  </si>
-  <si>
-    <t>Look for green verticall target. When you find it press SPACE bar. When the search array disappears click with mouse coursor where the target was. Press SPACE to start.</t>
+    <t>Look for green vertical target. When you find it press SPACE bar. When the search array disappears click with mouse coursor where the target was. If green vertical target is absent press on the white square in the right lower corner. Press SPACE to start.</t>
+  </si>
+  <si>
+    <t>Look for red horizontal target. When you find it press SPACE bar. When the search array disappears click with mouse coursor where the target was. If red horizontal target is absent press on the white square in the right lower corner. Press SPACE to start.</t>
   </si>
 </sst>
 </file>
@@ -414,7 +414,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,7 +438,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -449,7 +449,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>